<commit_message>
Update files via upload
Add future warning suppression and update Readme
</commit_message>
<xml_diff>
--- a/HousingPriceData/Results.xlsx
+++ b/HousingPriceData/Results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amber\Documents\GitHub\Capstone\Housing Price Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amber\Documents\GitHub\Capstone\HousingPriceData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AAF61EBE-7873-492F-A761-C4921977B662}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D43D604-5FBC-44CE-8BB8-BEF3956B5054}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5340" yWindow="1815" windowWidth="21435" windowHeight="13785" xr2:uid="{6C306806-C703-425E-9379-7979C7965D02}"/>
+    <workbookView xWindow="34530" yWindow="405" windowWidth="21435" windowHeight="13785" xr2:uid="{6C306806-C703-425E-9379-7979C7965D02}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="169" formatCode="&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -106,7 +106,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -368,13 +368,13 @@
                 <c:formatCode>"$"#,##0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>237577</c:v>
+                  <c:v>237908</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>295115</c:v>
+                  <c:v>295446</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>275115</c:v>
+                  <c:v>275446</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -748,13 +748,13 @@
                 <c:formatCode>"$"#,##0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>179403</c:v>
+                  <c:v>179072</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>236941</c:v>
+                  <c:v>236610</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>216941</c:v>
+                  <c:v>216610</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1853,7 +1853,7 @@
   <dimension ref="A3:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1867,7 +1867,7 @@
         <v>0</v>
       </c>
       <c r="B3">
-        <v>29087</v>
+        <v>29418</v>
       </c>
       <c r="D3">
         <v>20000</v>
@@ -1890,15 +1890,15 @@
       </c>
       <c r="B5" s="1">
         <f>B6+$B$3</f>
-        <v>237577</v>
+        <v>237908</v>
       </c>
       <c r="C5" s="1">
         <f>C6+$B$3</f>
-        <v>295115</v>
+        <v>295446</v>
       </c>
       <c r="D5" s="1">
         <f>C5-$D$3</f>
-        <v>275115</v>
+        <v>275446</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1922,15 +1922,15 @@
       </c>
       <c r="B7" s="1">
         <f>B6-$B$3</f>
-        <v>179403</v>
+        <v>179072</v>
       </c>
       <c r="C7" s="1">
         <f>C6-$B$3</f>
-        <v>236941</v>
+        <v>236610</v>
       </c>
       <c r="D7" s="1">
         <f t="shared" si="0"/>
-        <v>216941</v>
+        <v>216610</v>
       </c>
     </row>
   </sheetData>

</xml_diff>